<commit_message>
open points added in modules xlsx
</commit_message>
<xml_diff>
--- a/ERPNext Master Records.xlsx
+++ b/ERPNext Master Records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Master Records" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="593">
   <si>
     <t>MODULES</t>
   </si>
@@ -1815,6 +1815,9 @@
   </si>
   <si>
     <t>Document Share Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bug If we create Sales Invoice after sales order - tax info is not showing up correctly, If we create sales Invoice from get items from sales order way, It works </t>
   </si>
 </sst>
 </file>
@@ -1845,7 +1848,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1948,6 +1951,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1961,7 +1970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1981,6 +1990,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2263,7 +2273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2931,10 +2941,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A55"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2942,77 +2952,81 @@
     <col min="1" max="1" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
+      <c r="C5" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -3901,9 +3915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>